<commit_message>
updates Signed-off-by: Jace <jcmillett@xactware.com>
</commit_message>
<xml_diff>
--- a/UserImportURLs.xlsx
+++ b/UserImportURLs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="127">
   <si>
     <t>Base URL:</t>
   </si>
@@ -458,7 +458,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -467,6 +467,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -772,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -846,6 +849,9 @@
       <c r="G6" t="s">
         <v>121</v>
       </c>
+      <c r="I6" s="5" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -866,6 +872,9 @@
       <c r="H7" t="s">
         <v>122</v>
       </c>
+      <c r="I7" s="5" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
@@ -883,6 +892,12 @@
       <c r="H8" t="s">
         <v>122</v>
       </c>
+      <c r="I8" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I9" s="5"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -903,6 +918,9 @@
       <c r="G10" t="s">
         <v>121</v>
       </c>
+      <c r="I10" s="5" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -923,6 +941,9 @@
       <c r="G11" t="s">
         <v>124</v>
       </c>
+      <c r="I11" s="5" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -943,6 +964,7 @@
       <c r="G12" t="s">
         <v>124</v>
       </c>
+      <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
@@ -957,6 +979,7 @@
       <c r="G13" t="s">
         <v>124</v>
       </c>
+      <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -974,6 +997,10 @@
       <c r="G14" t="s">
         <v>124</v>
       </c>
+      <c r="I14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -991,8 +1018,9 @@
       <c r="F16" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I16" s="5"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>12</v>
       </c>
@@ -1005,8 +1033,9 @@
       <c r="F17" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I17" s="5"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>11</v>
       </c>
@@ -1022,8 +1051,9 @@
       <c r="F18" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I18" s="5"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>11</v>
       </c>
@@ -1036,8 +1066,9 @@
       <c r="F19" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I19" s="5"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>17</v>
       </c>
@@ -1047,8 +1078,9 @@
       <c r="F20" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>11</v>
       </c>
@@ -1058,8 +1090,9 @@
       <c r="F21" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I21" s="5"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>17</v>
       </c>
@@ -1069,8 +1102,12 @@
       <c r="F22" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I22" s="5"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I23" s="5"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>12</v>
       </c>
@@ -1083,8 +1120,9 @@
       <c r="F24" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I24" s="5"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>11</v>
       </c>
@@ -1100,8 +1138,9 @@
       <c r="F25" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I25" s="5"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>12</v>
       </c>
@@ -1114,8 +1153,9 @@
       <c r="F26" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I26" s="5"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>11</v>
       </c>
@@ -1128,8 +1168,9 @@
       <c r="F27" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I27" s="5"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>17</v>
       </c>
@@ -1139,8 +1180,9 @@
       <c r="F28" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I28" s="5"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>12</v>
       </c>
@@ -1153,8 +1195,9 @@
       <c r="F29" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I29" s="5"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>11</v>
       </c>
@@ -1164,8 +1207,9 @@
       <c r="F30" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I30" s="5"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>17</v>
       </c>
@@ -1175,8 +1219,12 @@
       <c r="F31" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I31" s="5"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I32" s="5"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>12</v>
       </c>
@@ -1189,8 +1237,9 @@
       <c r="F33" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I33" s="5"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>11</v>
       </c>
@@ -1200,8 +1249,9 @@
       <c r="F34" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I34" s="5"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>17</v>
       </c>
@@ -1211,8 +1261,12 @@
       <c r="F35" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I35" s="5"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I36" s="5"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>38</v>
       </c>
@@ -1225,8 +1279,9 @@
       <c r="F37" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I37" s="5"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>11</v>
       </c>
@@ -1239,8 +1294,9 @@
       <c r="F38" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I38" s="5"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>17</v>
       </c>
@@ -1253,8 +1309,12 @@
       <c r="F39" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I39" s="5"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I40" s="5"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>12</v>
       </c>
@@ -1267,8 +1327,9 @@
       <c r="F41" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I41" s="5"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>11</v>
       </c>
@@ -1281,8 +1342,9 @@
       <c r="F42" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I42" s="5"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>17</v>
       </c>
@@ -1295,8 +1357,12 @@
       <c r="F43" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I43" s="5"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I44" s="5"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>37</v>
       </c>
@@ -1315,8 +1381,11 @@
       <c r="G45" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I45" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>11</v>
       </c>
@@ -1335,8 +1404,9 @@
       <c r="G46" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I46" s="5"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>11</v>
       </c>
@@ -1352,8 +1422,9 @@
       <c r="G47" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I47" s="5"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>17</v>
       </c>
@@ -1363,8 +1434,9 @@
       <c r="F48" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I48" s="5"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>11</v>
       </c>
@@ -1374,8 +1446,9 @@
       <c r="F49" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I49" s="5"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>17</v>
       </c>
@@ -1385,8 +1458,12 @@
       <c r="F50" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I50" s="5"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I51" s="5"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>11</v>
       </c>
@@ -1402,8 +1479,9 @@
       <c r="F52" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I52" s="5"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>11</v>
       </c>
@@ -1416,8 +1494,9 @@
       <c r="F53" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I53" s="5"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>17</v>
       </c>
@@ -1427,8 +1506,9 @@
       <c r="F54" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I54" s="5"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>11</v>
       </c>
@@ -1438,8 +1518,9 @@
       <c r="F55" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I55" s="5"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>17</v>
       </c>
@@ -1449,8 +1530,12 @@
       <c r="F56" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I56" s="5"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I57" s="5"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>11</v>
       </c>
@@ -1466,8 +1551,9 @@
       <c r="F58" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I58" s="5"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>11</v>
       </c>
@@ -1480,8 +1566,9 @@
       <c r="F59" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I59" s="5"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>17</v>
       </c>
@@ -1491,8 +1578,9 @@
       <c r="F60" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I60" s="5"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>11</v>
       </c>
@@ -1502,8 +1590,9 @@
       <c r="F61" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I61" s="5"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>17</v>
       </c>
@@ -1513,8 +1602,12 @@
       <c r="F62" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I62" s="5"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I63" s="5"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>65</v>
       </c>
@@ -1530,8 +1623,9 @@
       <c r="F64" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I64" s="5"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>11</v>
       </c>
@@ -1544,8 +1638,9 @@
       <c r="G65" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I65" s="5"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>17</v>
       </c>
@@ -1558,8 +1653,12 @@
       <c r="G66" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I66" s="5"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I67" s="5"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>110</v>
       </c>
@@ -1575,8 +1674,9 @@
       <c r="F68" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I68" s="5"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>12</v>
       </c>
@@ -1589,8 +1689,9 @@
       <c r="F69" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I69" s="5"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>11</v>
       </c>
@@ -1603,8 +1704,9 @@
       <c r="F70" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I70" s="5"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>11</v>
       </c>
@@ -1614,8 +1716,9 @@
       <c r="F71" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I71" s="5"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>11</v>
       </c>
@@ -1625,6 +1728,7 @@
       <c r="F72" t="s">
         <v>119</v>
       </c>
+      <c r="I72" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1660,52 +1764,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CE18FB66DAA51F438814FC62671B832F" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="88c7f80eca5a8b22e0ba8d343359c654">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9b12015e-d264-48dc-9d22-f4372002aca2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="46c78192244aaf2a36493f5a8ba9a1dc" ns2:_="">
     <xsd:import namespace="9b12015e-d264-48dc-9d22-f4372002aca2"/>
@@ -1870,16 +1928,53 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="9b12015e-d264-48dc-9d22-f4372002aca2"/>
@@ -1895,15 +1990,16 @@
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51CB7F11-F939-4D6F-B6F0-5CEFE5772C64}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0664E4AD-3565-4F0E-A526-936D3B2C4EF3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1921,15 +2017,15 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E06D7A72-367C-4EBB-8CD9-01AF02A4CE5B}">
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51CB7F11-F939-4D6F-B6F0-5CEFE5772C64}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98A74783-91BB-4C12-870D-64739AC08013}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -1943,4 +2039,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E06D7A72-367C-4EBB-8CD9-01AF02A4CE5B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>